<commit_message>
added some figures to the proposal and added tet for busget section.
</commit_message>
<xml_diff>
--- a/proposal/budget/openFloatBudget.xlsx
+++ b/proposal/budget/openFloatBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebflaim/Documents/thesis/openFloat/proposal/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98AE50E-D657-AD4A-80D3-3DD9FD967C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B18B4-230F-3C41-B4E8-7BCE83A607DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{ED6DC47B-2186-CA44-BE05-803469EEC015}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{ED6DC47B-2186-CA44-BE05-803469EEC015}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,9 +343,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -364,6 +361,9 @@
     <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3854D8-F13F-B14F-89AD-0EA2FDF80B72}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="169" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="169" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -698,22 +698,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -722,19 +722,19 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="4">
         <v>7</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>0.5</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <f>C2*D2</f>
         <v>3.5</v>
       </c>
@@ -746,8 +746,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -756,7 +756,7 @@
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -768,8 +768,8 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -778,7 +778,7 @@
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -790,8 +790,8 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -800,7 +800,7 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -812,8 +812,8 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -822,7 +822,7 @@
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -834,8 +834,8 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -844,7 +844,7 @@
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>0.1</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -854,8 +854,8 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -864,7 +864,7 @@
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -874,33 +874,33 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <f>SUM(E2:E8)</f>
         <v>53.6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>19.95</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f>D10*C10</f>
         <v>39.9</v>
       </c>
@@ -913,17 +913,17 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>30</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <f>D11*C11</f>
         <v>30</v>
       </c>
@@ -933,17 +933,17 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>32.950000000000003</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <f>D12*C12</f>
         <v>32.950000000000003</v>
       </c>
@@ -956,17 +956,17 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>15</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <f>D13*C13</f>
         <v>15</v>
       </c>
@@ -976,34 +976,34 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <f>SUM(E10:E13)</f>
         <v>117.85000000000001</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>20</v>
       </c>
-      <c r="E15" s="10">
-        <f>D15*C15</f>
+      <c r="E15" s="9">
+        <f t="shared" ref="E15:E27" si="0">D15*C15</f>
         <v>20</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1012,18 +1012,18 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>2</v>
       </c>
-      <c r="E16" s="10">
-        <f>D16*C16</f>
+      <c r="E16" s="9">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1032,18 +1032,18 @@
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>8.9499999999999993</v>
       </c>
-      <c r="E17" s="10">
-        <f>D17*C17</f>
+      <c r="E17" s="9">
+        <f t="shared" si="0"/>
         <v>8.9499999999999993</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1055,18 +1055,18 @@
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>10</v>
       </c>
-      <c r="E18" s="10">
-        <f>D18*C18</f>
+      <c r="E18" s="9">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1078,18 +1078,18 @@
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E19" s="10">
-        <f>D19*C19</f>
+      <c r="E19" s="9">
+        <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1101,18 +1101,18 @@
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E20" s="10">
-        <f>D20*C20</f>
+      <c r="E20" s="9">
+        <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1124,18 +1124,18 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>6.95</v>
       </c>
-      <c r="E21" s="10">
-        <f>D21*C21</f>
+      <c r="E21" s="9">
+        <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1147,18 +1147,18 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>35</v>
       </c>
-      <c r="E22" s="10">
-        <f>D22*C22</f>
+      <c r="E22" s="9">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1170,18 +1170,18 @@
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="4">
         <v>2</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>30</v>
       </c>
-      <c r="E23" s="10">
-        <f>D23*C23</f>
+      <c r="E23" s="9">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1193,18 +1193,18 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="4">
         <v>2</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>20</v>
       </c>
-      <c r="E24" s="10">
-        <f>D24*C24</f>
+      <c r="E24" s="9">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1216,18 +1216,18 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>10</v>
       </c>
-      <c r="E25" s="10">
-        <f>D25*C25</f>
+      <c r="E25" s="9">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1239,18 +1239,18 @@
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="19"/>
+      <c r="B26" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>20</v>
       </c>
-      <c r="E26" s="10">
-        <f>D26*C26</f>
+      <c r="E26" s="9">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1262,18 +1262,18 @@
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="4">
         <v>2</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>10</v>
       </c>
-      <c r="E27" s="10">
-        <f>D27*C27</f>
+      <c r="E27" s="9">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1285,33 +1285,33 @@
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="11">
         <f>SUM(E15:E25)</f>
         <v>212.8</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>15</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <f>D29*C29</f>
         <v>15</v>
       </c>
@@ -1321,8 +1321,8 @@
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1331,7 +1331,7 @@
       <c r="D30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="9">
         <v>10</v>
       </c>
       <c r="F30" s="4" t="s">
@@ -1340,17 +1340,17 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="9">
         <v>10</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <f>C31*D31</f>
         <v>10</v>
       </c>
@@ -1360,17 +1360,17 @@
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <v>20</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <f>D32*C32</f>
         <v>20</v>
       </c>
@@ -1380,17 +1380,17 @@
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="4">
         <v>2</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>10</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <f>D33*C33</f>
         <v>20</v>
       </c>
@@ -1400,17 +1400,17 @@
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="14" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="4">
         <v>5</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <v>10</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="9">
         <f>D34*C34</f>
         <v>50</v>
       </c>
@@ -1420,8 +1420,8 @@
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -1430,7 +1430,7 @@
       <c r="D35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>20</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -1439,26 +1439,26 @@
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="11">
         <f>SUM(E29:E35)</f>
         <v>145</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="14"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="15">
         <f>SUM(B36, B28, B14, B9)</f>
         <v>529.25</v>
       </c>
@@ -1466,12 +1466,12 @@
     </row>
     <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="14"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="17">
         <f>SUMIF(F2:F35, "N", E2:E35)</f>
         <v>265</v>
       </c>

</xml_diff>